<commit_message>
now model can handle an extra layer and different learning rates
</commit_message>
<xml_diff>
--- a/DataSet/Resultados_estagio.xlsx
+++ b/DataSet/Resultados_estagio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Silva\Documents\Estágio 18\INESCTEC-FLYINGNETWORKS\DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6BCF2E-303C-44B9-BC44-5DB311CE3CF6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F747590B-EABD-457C-BBA9-691D545D3D0E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{FE193D26-1875-4712-B4F1-85F2BA6EC244}"/>
   </bookViews>
@@ -21,12 +21,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Scenario_Number</t>
   </si>
@@ -43,197 +48,50 @@
     <t>Throughput</t>
   </si>
   <si>
-    <t>3.4616623</t>
-  </si>
-  <si>
-    <t>228.88167</t>
-  </si>
-  <si>
-    <t>0.71827054</t>
-  </si>
-  <si>
-    <t>0.9750549999999999</t>
-  </si>
-  <si>
-    <t>166.3</t>
-  </si>
-  <si>
-    <t>3.026399</t>
-  </si>
-  <si>
-    <t>364.34045</t>
-  </si>
-  <si>
-    <t>5.487973</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
-    <t>7.3974724</t>
-  </si>
-  <si>
-    <t>565.83435</t>
-  </si>
-  <si>
-    <t>6.508517</t>
-  </si>
-  <si>
-    <t>721.8995</t>
-  </si>
-  <si>
-    <t>4.2647767</t>
-  </si>
-  <si>
-    <t>404.49908</t>
-  </si>
-  <si>
-    <t>5.2005954</t>
-  </si>
-  <si>
-    <t>400.12982</t>
-  </si>
-  <si>
-    <t>8.732895</t>
-  </si>
-  <si>
-    <t>435.64545</t>
-  </si>
-  <si>
-    <t>6.137148</t>
-  </si>
-  <si>
-    <t>576.7216</t>
-  </si>
-  <si>
-    <t>5.076104</t>
-  </si>
-  <si>
-    <t>452.9728</t>
-  </si>
-  <si>
-    <t>6.213237</t>
-  </si>
-  <si>
-    <t>478.3553</t>
-  </si>
-  <si>
-    <t>0.8981937999999999</t>
-  </si>
-  <si>
-    <t>462.6</t>
-  </si>
-  <si>
-    <t>4.549142000000001</t>
-  </si>
-  <si>
-    <t>0.622014</t>
-  </si>
-  <si>
-    <t>765.6</t>
-  </si>
-  <si>
-    <t>4.646988</t>
-  </si>
-  <si>
-    <t>6.090463000000001</t>
-  </si>
-  <si>
-    <t>617.9</t>
-  </si>
-  <si>
-    <t>0.7611860000000001</t>
-  </si>
-  <si>
-    <t>123.66666666666667</t>
-  </si>
-  <si>
-    <t>4.322381111111111</t>
-  </si>
-  <si>
-    <t>0.9301854444444443</t>
-  </si>
-  <si>
-    <t>0.9179215555555555</t>
-  </si>
-  <si>
-    <t>176.88888888888889</t>
-  </si>
-  <si>
-    <t>4.128777777777777</t>
-  </si>
-  <si>
-    <t>0.8589513333333333</t>
-  </si>
-  <si>
-    <t>517.1111111111111</t>
-  </si>
-  <si>
-    <t>8.23448777777778</t>
-  </si>
-  <si>
-    <t>0.7229115</t>
-  </si>
-  <si>
-    <t>785.3</t>
-  </si>
-  <si>
-    <t>4.855126</t>
-  </si>
-  <si>
-    <t>0.9230389000000001</t>
-  </si>
-  <si>
-    <t>221.3</t>
-  </si>
-  <si>
-    <t>5.147315000000001</t>
-  </si>
-  <si>
-    <t>0.8715022000000001</t>
-  </si>
-  <si>
-    <t>381.6</t>
-  </si>
-  <si>
-    <t>5.289137</t>
-  </si>
-  <si>
-    <t>75.0,105.0,225.0,105.0,135.0,225.0</t>
-  </si>
-  <si>
-    <t>105.0,75.0,75.0,255.0,225.0,165.0</t>
-  </si>
-  <si>
-    <t>105.0,225.0,105.0,75.0,225.0,135.0</t>
-  </si>
-  <si>
-    <t>195.0,105.0,75.0,135.0,165.0,225.0</t>
-  </si>
-  <si>
-    <t>75.0,195.0,165.0,45.0,195.0,225.0</t>
-  </si>
-  <si>
-    <t>195.0,45.0,75.0,165.0,195.0,225.0</t>
-  </si>
-  <si>
-    <t>135.0,225.0,75.0,75.0,255.0,75.0</t>
-  </si>
-  <si>
-    <t>75.0,75.0,135.0,255.0,255.0,75.0</t>
-  </si>
-  <si>
-    <t>225.0,165.0,75.0,75.0,75.0,255.0</t>
-  </si>
-  <si>
-    <t>225.0,135.0,75.0,75.0,105.0,225.0</t>
+    <t>X/Y of UAVS</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>75,0,105,0,225,0,105,0,135,0,225,0</t>
+  </si>
+  <si>
+    <t>105,0,225,0,105,0,75,0,225,0,135,0</t>
+  </si>
+  <si>
+    <t>195,0,105,0,75,0,135,0,165,0,225,0</t>
+  </si>
+  <si>
+    <t>75,0,195,0,165,0,45,0,195,0,225,0</t>
+  </si>
+  <si>
+    <t>195,0,45,0,75,0,165,0,195,0,225,0</t>
+  </si>
+  <si>
+    <t>135,0,225,0,75,0,75,0,255,0,75,0</t>
+  </si>
+  <si>
+    <t>75,0,75,0,135,0,255,0,255,0,75,0</t>
+  </si>
+  <si>
+    <t>225,0,165,0,75,0,75,0,75,0,255,0</t>
+  </si>
+  <si>
+    <t>225,0,135,0,75,0,75,0,105,0,225,0</t>
+  </si>
+  <si>
+    <t>105,0,75,0,75,0,255,0,225,0,165,0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +101,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -267,19 +132,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -591,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F20165-66F8-453A-8088-77B91CB660B4}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,7 +470,7 @@
     <col min="6" max="6" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,10 +478,16 @@
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -633,265 +507,385 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
+      <c r="C3">
+        <v>3.0263990000000001</v>
+      </c>
+      <c r="D3">
+        <v>166.3</v>
+      </c>
+      <c r="E3">
+        <v>0.97505499999999901</v>
+      </c>
+      <c r="G3">
+        <v>3.4616623</v>
+      </c>
+      <c r="H3">
+        <v>228.88167000000001</v>
+      </c>
+      <c r="I3">
+        <v>0.71827054000000001</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+      <c r="O3" s="4">
+        <f>(G3-C3)/C3</f>
+        <v>0.14382217942842299</v>
+      </c>
+      <c r="P3" s="4">
+        <f>(H3-D3)/D3</f>
+        <v>0.37631791942273002</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" ref="P3:Q12" si="0">(I3-E3)/E3</f>
+        <v>-0.26335382106650318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>7</v>
+      <c r="C4">
+        <v>4.5491419999999998</v>
+      </c>
+      <c r="D4">
+        <v>462.6</v>
+      </c>
+      <c r="E4">
+        <v>0.89819379999999904</v>
+      </c>
+      <c r="G4">
+        <v>5.4879730000000002</v>
+      </c>
+      <c r="H4">
+        <v>364.34044999999998</v>
+      </c>
+      <c r="I4">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" ref="O4:O12" si="1">(G4-C4)/C4</f>
+        <v>0.20637540002048749</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.21240715520968448</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.2003167467867171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>7</v>
+      <c r="C5">
+        <v>4.6469880000000003</v>
+      </c>
+      <c r="D5">
+        <v>765.6</v>
+      </c>
+      <c r="E5">
+        <v>0.62201399999999996</v>
+      </c>
+      <c r="G5">
+        <v>7.3974723999999998</v>
+      </c>
+      <c r="H5">
+        <v>565.83434999999997</v>
+      </c>
+      <c r="I5">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.59188541050676247</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.26092692006269597</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15474979662837182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>7</v>
+      <c r="C6">
+        <v>6.0904629999999997</v>
+      </c>
+      <c r="D6">
+        <v>617.9</v>
+      </c>
+      <c r="E6">
+        <v>0.76118600000000003</v>
+      </c>
+      <c r="G6">
+        <v>6.5085170000000003</v>
+      </c>
+      <c r="H6">
+        <v>721.89949999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="1"/>
+        <v>6.8640758510477878E-2</v>
+      </c>
+      <c r="P6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.16831121540702382</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.63797284763514E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>7</v>
+      <c r="C7" s="2">
+        <v>4.3223811111111097</v>
+      </c>
+      <c r="D7">
+        <v>123.666666666666</v>
+      </c>
+      <c r="E7">
+        <v>0.93018544444444395</v>
+      </c>
+      <c r="G7">
+        <v>4.2647766999999996</v>
+      </c>
+      <c r="H7">
+        <v>404.49907999999999</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.3327008801475691E-2</v>
+      </c>
+      <c r="P7" s="4">
+        <f t="shared" si="0"/>
+        <v>2.2708820485175378</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.22782006073101987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>7</v>
+      <c r="C8">
+        <v>4.1287777777777697</v>
+      </c>
+      <c r="D8">
+        <v>176.888888888888</v>
+      </c>
+      <c r="E8">
+        <v>0.91792155555555499</v>
+      </c>
+      <c r="G8">
+        <v>5.2005954000000001</v>
+      </c>
+      <c r="H8">
+        <v>400.12982</v>
+      </c>
+      <c r="I8">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.25959682983934157</v>
+      </c>
+      <c r="P8" s="4">
+        <f t="shared" si="0"/>
+        <v>1.2620404396985037</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.21750335238038931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" t="s">
-        <v>7</v>
+      <c r="C9">
+        <v>8.2344877777777796</v>
+      </c>
+      <c r="D9" s="2">
+        <v>517.11111111111097</v>
+      </c>
+      <c r="E9">
+        <v>0.85895133333333296</v>
+      </c>
+      <c r="G9">
+        <v>8.7328949999999992</v>
+      </c>
+      <c r="H9">
+        <v>435.64544999999998</v>
+      </c>
+      <c r="I9">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="1"/>
+        <v>6.0526803326766666E-2</v>
+      </c>
+      <c r="P9" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.15753995487752451</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.1637820303362158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" t="s">
-        <v>7</v>
+      <c r="C10">
+        <v>4.8551260000000003</v>
+      </c>
+      <c r="D10">
+        <v>785.3</v>
+      </c>
+      <c r="E10">
+        <v>0.72291150000000004</v>
+      </c>
+      <c r="G10">
+        <v>6.1371479999999998</v>
+      </c>
+      <c r="H10">
+        <v>576.72159999999997</v>
+      </c>
+      <c r="I10">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.26405535098368188</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.26560346364446707</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.4198176401952757E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" t="s">
-        <v>7</v>
+      <c r="C11">
+        <v>5.1473149999999999</v>
+      </c>
+      <c r="D11">
+        <v>221.3</v>
+      </c>
+      <c r="E11">
+        <v>0.9230389</v>
+      </c>
+      <c r="G11">
+        <v>5.0761039999999999</v>
+      </c>
+      <c r="H11">
+        <v>452.97280000000001</v>
+      </c>
+      <c r="I11">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.3834591432620679E-2</v>
+      </c>
+      <c r="P11" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0468721192950745</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.22184152802227511</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" t="s">
-        <v>7</v>
+      <c r="C12">
+        <v>5.2891370000000002</v>
+      </c>
+      <c r="D12">
+        <v>381.6</v>
+      </c>
+      <c r="E12">
+        <v>0.8715022</v>
+      </c>
+      <c r="G12">
+        <v>6.2132370000000003</v>
+      </c>
+      <c r="H12">
+        <v>478.3553</v>
+      </c>
+      <c r="I12">
+        <v>0.71827054000000001</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>17</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.17471659365223477</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2535516247379454</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.17582475408553183</v>
       </c>
     </row>
   </sheetData>
@@ -925,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
More results added to pdf
</commit_message>
<xml_diff>
--- a/DataSet/Resultados_estagio.xlsx
+++ b/DataSet/Resultados_estagio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Silva\Documents\Estágio 18\INESCTEC-FLYINGNETWORKS\DataSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F747590B-EABD-457C-BBA9-691D545D3D0E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98C081B-CC81-4CDC-8E97-23852E870CFD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{FE193D26-1875-4712-B4F1-85F2BA6EC244}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" activeTab="1" xr2:uid="{FE193D26-1875-4712-B4F1-85F2BA6EC244}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Scenario_Number</t>
   </si>
@@ -85,6 +85,36 @@
   </si>
   <si>
     <t>105,0,75,0,75,0,255,0,225,0,165,0</t>
+  </si>
+  <si>
+    <t>135,0;285,0|15,0;105,0|285,0;75,0|</t>
+  </si>
+  <si>
+    <t>285,0;105,0|135,0;285,0|45,0;105,0|</t>
+  </si>
+  <si>
+    <t>135,0;285,0|285,0;105,0|15,0;45,0|</t>
+  </si>
+  <si>
+    <t>135,0;105,0|135,0;285,0|195,0;135,0|</t>
+  </si>
+  <si>
+    <t>165,0;165,0|135,0:135,0|165,0;135,0|</t>
+  </si>
+  <si>
+    <t>165,0;195,0|135,0;135,0|135,0;105,0|</t>
+  </si>
+  <si>
+    <t>135,0;135,0|165,0;135,0|165,0;135,0|</t>
+  </si>
+  <si>
+    <t>135,0;135,0|165,0;165,0|135,0;165,0|</t>
+  </si>
+  <si>
+    <t>165,0;165,0|165,0;165,0|135,0;135,0|</t>
+  </si>
+  <si>
+    <t>135,0;135,0|135,0;165,0|165,0;165,0|</t>
   </si>
 </sst>
 </file>
@@ -136,13 +166,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -461,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F20165-66F8-453A-8088-77B91CB660B4}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -533,15 +560,15 @@
       <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="3">
         <f>(G3-C3)/C3</f>
         <v>0.14382217942842299</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <f>(H3-D3)/D3</f>
         <v>0.37631791942273002</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="3">
         <f t="shared" ref="P3:Q12" si="0">(I3-E3)/E3</f>
         <v>-0.26335382106650318</v>
       </c>
@@ -571,15 +598,15 @@
       <c r="K4" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <f t="shared" ref="O4:O12" si="1">(G4-C4)/C4</f>
         <v>0.20637540002048749</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <f t="shared" si="0"/>
         <v>-0.21240715520968448</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <f t="shared" si="0"/>
         <v>-0.2003167467867171</v>
       </c>
@@ -609,15 +636,15 @@
       <c r="K5" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <f t="shared" si="1"/>
         <v>0.59188541050676247</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="3">
         <f t="shared" si="0"/>
         <v>-0.26092692006269597</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <f t="shared" si="0"/>
         <v>0.15474979662837182</v>
       </c>
@@ -647,15 +674,15 @@
       <c r="K6" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <f t="shared" si="1"/>
         <v>6.8640758510477878E-2</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <f t="shared" si="0"/>
         <v>0.16831121540702382</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <f t="shared" si="0"/>
         <v>-5.63797284763514E-2</v>
       </c>
@@ -685,15 +712,15 @@
       <c r="K7" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <f t="shared" si="1"/>
         <v>-1.3327008801475691E-2</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <f t="shared" si="0"/>
         <v>2.2708820485175378</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <f t="shared" si="0"/>
         <v>-0.22782006073101987</v>
       </c>
@@ -723,15 +750,15 @@
       <c r="K8" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="3">
         <f t="shared" si="1"/>
         <v>0.25959682983934157</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="3">
         <f t="shared" si="0"/>
         <v>1.2620404396985037</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <f t="shared" si="0"/>
         <v>-0.21750335238038931</v>
       </c>
@@ -761,15 +788,15 @@
       <c r="K9" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="3">
         <f t="shared" si="1"/>
         <v>6.0526803326766666E-2</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <f t="shared" si="0"/>
         <v>-0.15753995487752451</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <f t="shared" si="0"/>
         <v>-0.1637820303362158</v>
       </c>
@@ -799,15 +826,15 @@
       <c r="K10" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="3">
         <f t="shared" si="1"/>
         <v>0.26405535098368188</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="3">
         <f t="shared" si="0"/>
         <v>-0.26560346364446707</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <f t="shared" si="0"/>
         <v>-6.4198176401952757E-3</v>
       </c>
@@ -837,15 +864,15 @@
       <c r="K11" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="3">
         <f t="shared" si="1"/>
         <v>-1.3834591432620679E-2</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="3">
         <f t="shared" si="0"/>
         <v>1.0468721192950745</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <f t="shared" si="0"/>
         <v>-0.22184152802227511</v>
       </c>
@@ -875,15 +902,15 @@
       <c r="K12" t="s">
         <v>17</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12" s="3">
         <f t="shared" si="1"/>
         <v>0.17471659365223477</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="3">
         <f t="shared" si="0"/>
         <v>0.2535516247379454</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <f t="shared" si="0"/>
         <v>-0.17582475408553183</v>
       </c>
@@ -896,10 +923,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE1DAF4-3521-4095-92EB-6479CD5FE6B8}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,89 +938,431 @@
     <col min="8" max="8" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C2" s="3" t="s">
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>3.0037699999999998</v>
+      </c>
+      <c r="D3">
+        <v>170.2</v>
+      </c>
+      <c r="E3">
+        <v>0.96318839999999994</v>
+      </c>
+      <c r="G3">
+        <v>3.0737182999999999</v>
+      </c>
+      <c r="H3">
+        <v>264.91622999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.82127106000000005</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="3">
+        <f>(G3-C3)/C3</f>
+        <v>2.3286836209163844E-2</v>
+      </c>
+      <c r="P3" s="3">
+        <f t="shared" ref="P3:Q12" si="0">(H3-D3)/D3</f>
+        <v>0.55649958871915395</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.14734120552116273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>4.0638889999999996</v>
+      </c>
+      <c r="D4">
+        <v>346.5</v>
+      </c>
+      <c r="E4">
+        <v>0.88687959999999999</v>
+      </c>
+      <c r="G4">
+        <v>4.3420290000000001</v>
+      </c>
+      <c r="H4">
+        <v>237.07744</v>
+      </c>
+      <c r="I4">
+        <v>0.76886182999999997</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="3">
+        <f t="shared" ref="O4:O12" si="1">(G4-C4)/C4</f>
+        <v>6.8441829981084751E-2</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.31579382395382399</v>
+      </c>
+      <c r="Q4" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.13307079111978676</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>5.4717419999999999</v>
+      </c>
+      <c r="D5">
+        <v>817</v>
+      </c>
+      <c r="E5">
+        <v>0.66015599999999997</v>
+      </c>
+      <c r="G5">
+        <v>6.996105</v>
+      </c>
+      <c r="H5">
+        <v>434.87853999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.81902050000000004</v>
+      </c>
+      <c r="K5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.27858824484049144</v>
+      </c>
+      <c r="P5" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.46771292533659731</v>
+      </c>
+      <c r="Q5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.24064690770060423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>5.6174979999999897</v>
+      </c>
+      <c r="D6">
+        <v>714.3</v>
+      </c>
+      <c r="E6">
+        <v>0.70148519999999903</v>
+      </c>
+      <c r="G6">
+        <v>5.0547743000000001</v>
+      </c>
+      <c r="H6">
+        <v>354.36502000000002</v>
+      </c>
+      <c r="I6">
+        <v>0.82701069999999999</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="3">
+        <f t="shared" si="1"/>
+        <v>-0.10017336899808253</v>
+      </c>
+      <c r="P6" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.50389889402211951</v>
+      </c>
+      <c r="Q6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.17894247804515495</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C7" s="2">
+        <v>4.1906999999999996</v>
+      </c>
+      <c r="D7">
+        <v>683.33333333333303</v>
+      </c>
+      <c r="E7">
+        <v>0.81491311111111098</v>
+      </c>
+      <c r="G7">
+        <v>4.3258032999999996</v>
+      </c>
+      <c r="H7">
+        <v>290.72894000000002</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.6764133</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="1"/>
+        <v>3.2238838380222859E-2</v>
+      </c>
+      <c r="P7" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.57454301463414614</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.1699565379703738</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>4.7287289999999897</v>
+      </c>
+      <c r="D8">
+        <v>291.5</v>
+      </c>
+      <c r="E8">
+        <v>0.91456459999999995</v>
+      </c>
+      <c r="G8">
+        <v>4.2624725999999997</v>
+      </c>
+      <c r="H8">
+        <v>479.36806999999999</v>
+      </c>
+      <c r="I8">
+        <v>0.72260610000000003</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="1"/>
+        <v>-9.860078680761597E-2</v>
+      </c>
+      <c r="P8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64448737564322467</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.20989058618713202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>3.1043239999999899</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1074.4000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.4704834</v>
+      </c>
+      <c r="G9">
+        <v>5.6644363000000002</v>
+      </c>
+      <c r="H9">
+        <v>235.89975000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.82134414</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.82469236458566142</v>
+      </c>
+      <c r="P9" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.78043582464631422</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.74574520588824178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>5.4535749999999998</v>
+      </c>
+      <c r="D10">
+        <v>942.7</v>
+      </c>
+      <c r="E10">
+        <v>0.73875829999999998</v>
+      </c>
+      <c r="G10">
+        <v>5.3590470000000003</v>
+      </c>
+      <c r="H10">
+        <v>672.41223000000002</v>
+      </c>
+      <c r="I10">
+        <v>0.75247920000000001</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="1"/>
+        <v>-1.7333217201560353E-2</v>
+      </c>
+      <c r="P10" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.2867166330752095</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8572921617259711E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>2.9972650000000001</v>
+      </c>
+      <c r="D11">
+        <v>1047.8</v>
+      </c>
+      <c r="E11">
+        <v>0.64688489999999998</v>
+      </c>
+      <c r="G11">
+        <v>4.7074503999999999</v>
+      </c>
+      <c r="H11">
+        <v>62.626750000000001</v>
+      </c>
+      <c r="I11">
+        <v>0.71508366000000001</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.57058198057228837</v>
+      </c>
+      <c r="P11" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.94023024432143532</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1054264212999871</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
+      </c>
+      <c r="C12">
+        <v>4.4238977777777704</v>
+      </c>
+      <c r="D12">
+        <v>584.33333333333303</v>
+      </c>
+      <c r="E12">
+        <v>0.77470677777777697</v>
+      </c>
+      <c r="G12">
+        <v>5.2027919999999996</v>
+      </c>
+      <c r="H12">
+        <v>296.96575999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.69313157000000003</v>
+      </c>
+      <c r="K12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.17606514918468266</v>
+      </c>
+      <c r="P12" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.49178706217912127</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" si="0"/>
+        <v>-0.10529817231207524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>